<commit_message>
Modified weights and draw.io model
</commit_message>
<xml_diff>
--- a/weights.xlsx
+++ b/weights.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Mobius\wpa-attacks-modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FCF355-F063-4B24-85BD-BD0CB5C6F86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F99EDED-1784-4B50-A8D9-C0696D311DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1692" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{163A671C-54E9-454C-BAF3-1E42CFA22378}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Attack</t>
   </si>
@@ -81,9 +81,6 @@
     <t>SENSITIVE INFO</t>
   </si>
   <si>
-    <t>Detectability</t>
-  </si>
-  <si>
     <t>Network Layer Attack</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>hasHW</t>
   </si>
   <si>
-    <t>hasPhysical</t>
-  </si>
-  <si>
     <t>Sensitive Info</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Expected Outcome</t>
   </si>
   <si>
-    <t>DOS via packet forging and social engineering</t>
-  </si>
-  <si>
     <t>Scan Network</t>
   </si>
   <si>
@@ -171,17 +162,26 @@
     <t>INFO via social eng</t>
   </si>
   <si>
-    <t xml:space="preserve">INFO via MITM and social eng </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOS via MITM and rogue AP || social eng </t>
+    <t>DOS via packet forging and social eng.</t>
+  </si>
+  <si>
+    <t>Detectability Success</t>
+  </si>
+  <si>
+    <t>Detectability Failure</t>
+  </si>
+  <si>
+    <t>INFO via MITM and social eng.</t>
+  </si>
+  <si>
+    <t>DOS via MITM social eng.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +211,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +281,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -388,10 +412,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -402,16 +428,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -429,17 +452,52 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -681,24 +739,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E89D574-E88C-47BF-90B6-2FB608C0DD7A}" name="Table1" displayName="Table1" ref="D3:G11" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="D3:G11" xr:uid="{5E89D574-E88C-47BF-90B6-2FB608C0DD7A}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E416DAE3-E73A-4059-AF85-003B716B63B3}" name="Attack" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A9391208-A0C5-4324-AABA-BAA713FDD3BE}" name="Attack Cost" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1DED7961-A603-4878-B4A7-359BF8777937}" name="Time" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{0E2EAE03-3319-43B4-91C4-E2DB2D1E8B0C}" name="Detectability" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E89D574-E88C-47BF-90B6-2FB608C0DD7A}" name="Table1" displayName="Table1" ref="D3:H11" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="D3:H11" xr:uid="{5E89D574-E88C-47BF-90B6-2FB608C0DD7A}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E416DAE3-E73A-4059-AF85-003B716B63B3}" name="Attack" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A9391208-A0C5-4324-AABA-BAA713FDD3BE}" name="Attack Cost" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{1DED7961-A603-4878-B4A7-359BF8777937}" name="Time" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{0E2EAE03-3319-43B4-91C4-E2DB2D1E8B0C}" name="Detectability Success" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{54264172-334C-47A8-AA68-E8FCB59BC937}" name="Detectability Failure" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}" name="Table3" displayName="Table3" ref="I3:J5" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="I3:J5" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}" name="Table3" displayName="Table3" ref="E16:F18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="E16:F18" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CE3A79F0-85C8-4AC3-8B79-6012262499B7}" name="Goal" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{665CCBC3-3834-455C-8DAB-54F98F202DA3}" name="Payoff" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CE3A79F0-85C8-4AC3-8B79-6012262499B7}" name="Goal" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{665CCBC3-3834-455C-8DAB-54F98F202DA3}" name="Payoff" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1001,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED30BE9-7035-40CA-ACCD-8F9DDAB93A26}">
-  <dimension ref="D3:J11"/>
+  <dimension ref="D3:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H11" sqref="D3:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,8 +1074,8 @@
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" customWidth="1"/>
@@ -1032,7 +1091,7 @@
     <col min="23" max="23" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,17 +1102,14 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="7">
@@ -1065,15 +1121,12 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="7">
@@ -1083,17 +1136,14 @@
         <v>10</v>
       </c>
       <c r="G5" s="4">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="25" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="7">
@@ -1103,11 +1153,14 @@
         <v>6</v>
       </c>
       <c r="G6" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="3" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="25" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7">
@@ -1117,11 +1170,14 @@
         <v>8</v>
       </c>
       <c r="G7" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="7">
@@ -1131,12 +1187,15 @@
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="25" t="s">
+        <v>14</v>
       </c>
       <c r="E9" s="7">
         <v>4</v>
@@ -1145,11 +1204,14 @@
         <v>4</v>
       </c>
       <c r="G9" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="3" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="25" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="7">
@@ -1159,11 +1221,14 @@
         <v>2</v>
       </c>
       <c r="G10" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="5" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="26" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="9">
@@ -1173,7 +1238,34 @@
         <v>7</v>
       </c>
       <c r="G11" s="6">
-        <v>6</v>
+        <v>0.3</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1189,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0165ADE4-AA4B-4DA6-B0DA-4E74F7888BB2}">
-  <dimension ref="C7:M25"/>
+  <dimension ref="C7:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,159 +1293,161 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="40.5703125" customWidth="1"/>
+    <col min="12" max="12" width="38.140625" customWidth="1"/>
+    <col min="13" max="13" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="H7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="I7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="12">
+        <v>200</v>
+      </c>
+      <c r="K8" s="24">
+        <v>36</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>4</v>
-      </c>
-      <c r="F8" s="10">
-        <v>7</v>
-      </c>
-      <c r="G8" s="10">
-        <v>8</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="12">
-        <v>500</v>
-      </c>
-      <c r="K8" s="12">
-        <v>500</v>
-      </c>
-      <c r="L8" s="13">
-        <v>81</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="20" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" s="10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="10">
         <v>0</v>
       </c>
       <c r="G9" s="10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H9" s="11">
         <v>1</v>
       </c>
-      <c r="I9" s="11">
-        <v>1</v>
+      <c r="I9" s="12">
+        <v>1000</v>
       </c>
       <c r="J9" s="12">
-        <v>1000</v>
-      </c>
-      <c r="K9" s="12">
         <v>200</v>
       </c>
-      <c r="L9" s="12">
-        <v>104</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>37</v>
+      <c r="K9" s="20">
+        <v>56</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="20" t="s">
-        <v>26</v>
+      <c r="C10" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
         <v>10</v>
-      </c>
-      <c r="E10" s="10">
-        <v>9</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0</v>
       </c>
       <c r="G10" s="10">
         <v>10</v>
       </c>
       <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1000</v>
       </c>
       <c r="J10" s="12">
-        <v>1000</v>
-      </c>
-      <c r="K10" s="12">
         <v>200</v>
       </c>
-      <c r="L10" s="12">
-        <v>168</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>35</v>
+      <c r="K10" s="20">
+        <v>57</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="20" t="s">
-        <v>27</v>
+      <c r="C11" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="D11" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
@@ -1364,31 +1458,31 @@
       <c r="H11" s="11">
         <v>1</v>
       </c>
-      <c r="I11" s="11">
-        <v>1</v>
+      <c r="I11" s="12">
+        <v>200</v>
       </c>
       <c r="J11" s="12">
-        <v>200</v>
-      </c>
-      <c r="K11" s="12">
         <v>1000</v>
       </c>
-      <c r="L11" s="12">
-        <v>216</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>34</v>
+      <c r="K11" s="20">
+        <v>72</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="20" t="s">
-        <v>28</v>
+      <c r="C12" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="D12" s="10">
         <v>10</v>
       </c>
       <c r="E12" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
@@ -1399,60 +1493,60 @@
       <c r="H12" s="11">
         <v>1</v>
       </c>
-      <c r="I12" s="11">
-        <v>1</v>
+      <c r="I12" s="12">
+        <v>200</v>
       </c>
       <c r="J12" s="12">
-        <v>200</v>
-      </c>
-      <c r="K12" s="12">
         <v>1000</v>
       </c>
-      <c r="L12" s="12">
-        <v>264</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>36</v>
+      <c r="K12" s="20">
+        <v>88</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="20" t="s">
-        <v>29</v>
+      <c r="C13" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="11">
         <v>1</v>
       </c>
-      <c r="I13" s="11">
-        <v>1</v>
+      <c r="I13" s="12">
+        <v>1000</v>
       </c>
       <c r="J13" s="12">
         <v>1000</v>
       </c>
-      <c r="K13" s="12">
-        <v>1000</v>
-      </c>
-      <c r="L13" s="12">
-        <v>289</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>41</v>
+      <c r="K13" s="20">
+        <v>99</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="20" t="s">
-        <v>30</v>
+      <c r="C14" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="D14" s="10">
         <v>10</v>
@@ -1469,98 +1563,125 @@
       <c r="H14" s="11">
         <v>1</v>
       </c>
-      <c r="I14" s="11">
-        <v>1</v>
+      <c r="I14" s="12">
+        <v>1000</v>
       </c>
       <c r="J14" s="12">
         <v>1000</v>
       </c>
-      <c r="K14" s="12">
-        <v>1000</v>
-      </c>
-      <c r="L14" s="12">
-        <v>289</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18" s="18" t="s">
+      <c r="K14" s="20">
+        <v>128</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L19" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="19" t="s">
+      <c r="M22" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L20" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L21" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L22" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L24" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="19" t="s">
+      <c r="M26" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L25" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M25" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C8:M14">
+    <sortCondition ref="K7:K14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8a9b620c-34c6-4e2c-9301-6ea45fc12233" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1747,17 +1868,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8a9b620c-34c6-4e2c-9301-6ea45fc12233" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16FEDAB8-E425-4256-822B-CE907893B817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62920E99-3B4A-4A2F-B79C-84ADA3E750BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8a9b620c-34c6-4e2c-9301-6ea45fc12233"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7bd399c7-d5a3-450d-b631-6b4334870a0b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1782,18 +1913,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62920E99-3B4A-4A2F-B79C-84ADA3E750BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16FEDAB8-E425-4256-822B-CE907893B817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8a9b620c-34c6-4e2c-9301-6ea45fc12233"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7bd399c7-d5a3-450d-b631-6b4334870a0b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added overall attack graph in draw.io
</commit_message>
<xml_diff>
--- a/weights.xlsx
+++ b/weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Mobius\wpa-attacks-modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F99EDED-1784-4B50-A8D9-C0696D311DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF0D204-0150-4384-A62C-35715A83F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1692" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{163A671C-54E9-454C-BAF3-1E42CFA22378}"/>
   </bookViews>
@@ -181,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,15 +218,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,11 +279,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -412,12 +400,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -467,17 +454,13 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -494,22 +477,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -584,6 +551,22 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -746,18 +729,18 @@
     <tableColumn id="2" xr3:uid="{A9391208-A0C5-4324-AABA-BAA713FDD3BE}" name="Attack Cost" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{1DED7961-A603-4878-B4A7-359BF8777937}" name="Time" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{0E2EAE03-3319-43B4-91C4-E2DB2D1E8B0C}" name="Detectability Success" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{54264172-334C-47A8-AA68-E8FCB59BC937}" name="Detectability Failure" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{54264172-334C-47A8-AA68-E8FCB59BC937}" name="Detectability Failure" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}" name="Table3" displayName="Table3" ref="E16:F18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}" name="Table3" displayName="Table3" ref="E16:F18" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="E16:F18" xr:uid="{B30C1D52-C765-46E8-9801-7B4D45F704A7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CE3A79F0-85C8-4AC3-8B79-6012262499B7}" name="Goal" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{665CCBC3-3834-455C-8DAB-54F98F202DA3}" name="Payoff" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CE3A79F0-85C8-4AC3-8B79-6012262499B7}" name="Goal" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{665CCBC3-3834-455C-8DAB-54F98F202DA3}" name="Payoff" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,7 +1092,7 @@
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="7">
@@ -1126,7 +1109,7 @@
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="7">
@@ -1143,7 +1126,7 @@
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="7">
@@ -1160,7 +1143,7 @@
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7">
@@ -1177,7 +1160,7 @@
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="7">
@@ -1194,7 +1177,7 @@
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="7">
@@ -1211,7 +1194,7 @@
       </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="7">
@@ -1228,7 +1211,7 @@
       </c>
     </row>
     <row r="11" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="9">
@@ -1359,7 +1342,7 @@
       <c r="J8" s="12">
         <v>200</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="23">
         <v>36</v>
       </c>
       <c r="L8" s="18" t="s">
@@ -1505,7 +1488,7 @@
       <c r="L12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1641,7 +1624,7 @@
       <c r="L24" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1677,11 +1660,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8a9b620c-34c6-4e2c-9301-6ea45fc12233" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1868,27 +1852,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8a9b620c-34c6-4e2c-9301-6ea45fc12233" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62920E99-3B4A-4A2F-B79C-84ADA3E750BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16FEDAB8-E425-4256-822B-CE907893B817}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8a9b620c-34c6-4e2c-9301-6ea45fc12233"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7bd399c7-d5a3-450d-b631-6b4334870a0b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1913,9 +1887,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16FEDAB8-E425-4256-822B-CE907893B817}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62920E99-3B4A-4A2F-B79C-84ADA3E750BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8a9b620c-34c6-4e2c-9301-6ea45fc12233"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7bd399c7-d5a3-450d-b631-6b4334870a0b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>